<commit_message>
Finalized and Proofread Tax Evasion Story
</commit_message>
<xml_diff>
--- a/Stories/TaxEvasion.xlsx
+++ b/Stories/TaxEvasion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ianch\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C899C9D7-FC2E-4192-84C7-21F081672C4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA66968-D52F-49A4-9602-84C1DED3BE7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{828238F6-C267-4DF0-864C-89635999C88D}"/>
   </bookViews>
@@ -309,7 +309,7 @@
     <t>We could negeotiate with the general to reduce his sentences if he expose any other confederates.</t>
   </si>
   <si>
-    <t>What if he pay some fancy money to the council to defend him? No! I say we make him walk around and give us all our shares.</t>
+    <t>What if he pay some fancy money to the council that will defend him? No! I say we make him walk around and give us all our shares.</t>
   </si>
 </sst>
 </file>
@@ -524,11 +524,17 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -537,12 +543,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -862,37 +862,37 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1"/>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="19" t="s">
+      <c r="C1" s="13"/>
+      <c r="D1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="14"/>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="19" t="s">
+      <c r="G1" s="13"/>
+      <c r="H1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="19" t="s">
+      <c r="I1" s="13"/>
+      <c r="J1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="14"/>
-      <c r="L1" s="19" t="s">
+      <c r="K1" s="13"/>
+      <c r="L1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="14"/>
+      <c r="M1" s="13"/>
     </row>
     <row r="2" spans="1:13" ht="41.4">
       <c r="A2" s="2"/>
@@ -937,39 +937,39 @@
       <c r="A3" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="13"/>
-      <c r="L3" s="13"/>
-      <c r="M3" s="14"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="13"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1">
       <c r="A4" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
-      <c r="L4" s="13"/>
-      <c r="M4" s="14"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
+      <c r="I4" s="16"/>
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="13"/>
     </row>
     <row r="5" spans="1:13" ht="193.2">
       <c r="A5" s="7" t="s">
@@ -1016,39 +1016,39 @@
       <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
-      <c r="K6" s="13"/>
-      <c r="L6" s="13"/>
-      <c r="M6" s="14"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="13"/>
     </row>
     <row r="7" spans="1:13" ht="27.6">
       <c r="A7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="13"/>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="14"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
+      <c r="J7" s="16"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="13"/>
     </row>
     <row r="8" spans="1:13" ht="220.8">
       <c r="A8" s="7" t="s">
@@ -1095,22 +1095,22 @@
       <c r="A9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
-      <c r="M9" s="14"/>
-    </row>
-    <row r="10" spans="1:13" ht="220.8">
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="13"/>
+    </row>
+    <row r="10" spans="1:13" ht="207">
       <c r="A10" s="7" t="s">
         <v>18</v>
       </c>
@@ -1155,20 +1155,20 @@
       <c r="A11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="13"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="13"/>
-      <c r="L11" s="13"/>
-      <c r="M11" s="14"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="16"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="K11" s="16"/>
+      <c r="L11" s="16"/>
+      <c r="M11" s="13"/>
     </row>
     <row r="12" spans="1:13" ht="193.2">
       <c r="A12" s="7" t="s">
@@ -1215,20 +1215,20 @@
       <c r="A13" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="13"/>
-      <c r="M13" s="14"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
+      <c r="M13" s="13"/>
     </row>
     <row r="14" spans="1:13" ht="248.4">
       <c r="A14" s="7" t="s">
@@ -1273,12 +1273,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
     <mergeCell ref="B11:M11"/>
     <mergeCell ref="B13:M13"/>
     <mergeCell ref="B3:M3"/>
@@ -1286,6 +1280,12 @@
     <mergeCell ref="B6:M6"/>
     <mergeCell ref="B7:M7"/>
     <mergeCell ref="B9:M9"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added event summary for TaxEvasion
</commit_message>
<xml_diff>
--- a/Stories/TaxEvasion.xlsx
+++ b/Stories/TaxEvasion.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ianch\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School Related\DECO3801\DECO3801-Synergistiscs\Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA66968-D52F-49A4-9602-84C1DED3BE7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49562AAA-F1F4-40D9-8DA9-C2029E547673}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{828238F6-C267-4DF0-864C-89635999C88D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{828238F6-C267-4DF0-864C-89635999C88D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="102">
   <si>
     <t>MILITARY</t>
   </si>
@@ -310,6 +310,36 @@
   </si>
   <si>
     <t>What if he pay some fancy money to the council that will defend him? No! I say we make him walk around and give us all our shares.</t>
+  </si>
+  <si>
+    <t>EVENT SUMMARY HEADER</t>
+  </si>
+  <si>
+    <t>ACTION 1 EVENT SUMMARY</t>
+  </si>
+  <si>
+    <t>ACTION 2 EVENT SUMMARY</t>
+  </si>
+  <si>
+    <t>ACTION 3 EVENT SUMMARY</t>
+  </si>
+  <si>
+    <t>ACTION 4 EVENT SUMMARY</t>
+  </si>
+  <si>
+    <t>It turns out the Military Commander had been selling Kingdom secrets to the neighbouring Kingdom and is given sums of gold from the neighbouring Kingdom, hence avoiding the tax payment.</t>
+  </si>
+  <si>
+    <t>This had sparked the neighbouring Kingdom to launch an attack on your Kingdom in order to save the Commander due to a pact he had made with the neighbouring Kingdom. This angered you and you decide to wage war on the neighbouring Kingdom.</t>
+  </si>
+  <si>
+    <t>The Military Commander was angered by this decision which lead him to betray the Kingdom and join the neighbouring Kingdom. The neighbouring Kingdom saw this as an opportunity to attack your Kingdom as you were without a Military Commander.</t>
+  </si>
+  <si>
+    <t>A sense of anger and betrayal was felt by the Military Commander due to this decision. This had made him sell Kingdom secrets to the neighbouring Kingdoms. However, you managed to prevent this from happening and executed him for treason.</t>
+  </si>
+  <si>
+    <t>Putting the Military Commander on trial made him confess that he had been selling Kingdom secrets to the neighbouring Kingdoms. He had been receiving gold for it, hence not paying taxes in order to avoid getting caught.</t>
   </si>
 </sst>
 </file>
@@ -489,7 +519,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -524,25 +554,28 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -859,40 +892,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E371D5D-5D35-41E8-9F5D-D5C6C509E3AF}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1"/>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="12" t="s">
+      <c r="C1" s="14"/>
+      <c r="D1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="F1" s="12" t="s">
+      <c r="E1" s="14"/>
+      <c r="F1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="12" t="s">
+      <c r="G1" s="14"/>
+      <c r="H1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="13"/>
-      <c r="J1" s="12" t="s">
+      <c r="I1" s="14"/>
+      <c r="J1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="13"/>
-      <c r="L1" s="12" t="s">
+      <c r="K1" s="14"/>
+      <c r="L1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="13"/>
+      <c r="M1" s="14"/>
     </row>
     <row r="2" spans="1:13" ht="41.4">
       <c r="A2" s="2"/>
@@ -933,43 +966,43 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="27.6">
+    <row r="3" spans="1:13" ht="34.799999999999997" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="16"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="16"/>
-      <c r="I3" s="16"/>
-      <c r="J3" s="16"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="16"/>
-      <c r="M3" s="13"/>
-    </row>
-    <row r="4" spans="1:13" ht="15" customHeight="1">
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="14"/>
+    </row>
+    <row r="4" spans="1:13" ht="38.4" customHeight="1">
       <c r="A4" s="9" t="b">
         <v>1</v>
       </c>
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="K4" s="16"/>
-      <c r="L4" s="16"/>
-      <c r="M4" s="13"/>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="14"/>
     </row>
     <row r="5" spans="1:13" ht="193.2">
       <c r="A5" s="7" t="s">
@@ -1016,39 +1049,39 @@
       <c r="A6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="13"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
+      <c r="M6" s="14"/>
     </row>
     <row r="7" spans="1:13" ht="27.6">
       <c r="A7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="16"/>
-      <c r="G7" s="16"/>
-      <c r="H7" s="16"/>
-      <c r="I7" s="16"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="16"/>
-      <c r="L7" s="16"/>
-      <c r="M7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
+      <c r="M7" s="14"/>
     </row>
     <row r="8" spans="1:13" ht="220.8">
       <c r="A8" s="7" t="s">
@@ -1095,20 +1128,20 @@
       <c r="A9" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
-      <c r="H9" s="16"/>
-      <c r="I9" s="16"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="13"/>
+      <c r="C9" s="13"/>
+      <c r="D9" s="13"/>
+      <c r="E9" s="13"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="13"/>
+      <c r="K9" s="13"/>
+      <c r="L9" s="13"/>
+      <c r="M9" s="14"/>
     </row>
     <row r="10" spans="1:13" ht="207">
       <c r="A10" s="7" t="s">
@@ -1155,20 +1188,20 @@
       <c r="A11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="16"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="16"/>
-      <c r="L11" s="16"/>
-      <c r="M11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="14"/>
     </row>
     <row r="12" spans="1:13" ht="193.2">
       <c r="A12" s="7" t="s">
@@ -1215,20 +1248,20 @@
       <c r="A13" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
-      <c r="L13" s="16"/>
-      <c r="M13" s="13"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="13"/>
+      <c r="L13" s="13"/>
+      <c r="M13" s="14"/>
     </row>
     <row r="14" spans="1:13" ht="248.4">
       <c r="A14" s="7" t="s">
@@ -1271,8 +1304,114 @@
         <v>63</v>
       </c>
     </row>
+    <row r="15" spans="1:13" ht="55.2">
+      <c r="A15" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
+      <c r="E15" s="13"/>
+      <c r="F15" s="13"/>
+      <c r="G15" s="13"/>
+      <c r="H15" s="13"/>
+      <c r="I15" s="13"/>
+      <c r="J15" s="13"/>
+      <c r="K15" s="13"/>
+      <c r="L15" s="13"/>
+      <c r="M15" s="14"/>
+    </row>
+    <row r="16" spans="1:13" ht="55.2">
+      <c r="A16" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="14"/>
+    </row>
+    <row r="17" spans="1:13" ht="55.2">
+      <c r="A17" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="14"/>
+    </row>
+    <row r="18" spans="1:13" ht="55.2">
+      <c r="A18" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B18" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="13"/>
+      <c r="D18" s="13"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="14"/>
+    </row>
+    <row r="19" spans="1:13" ht="55.2">
+      <c r="A19" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="20" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19" s="13"/>
+      <c r="D19" s="13"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="18">
+    <mergeCell ref="B15:M15"/>
+    <mergeCell ref="B16:M16"/>
+    <mergeCell ref="B17:M17"/>
+    <mergeCell ref="B18:M18"/>
+    <mergeCell ref="B19:M19"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
     <mergeCell ref="B11:M11"/>
     <mergeCell ref="B13:M13"/>
     <mergeCell ref="B3:M3"/>
@@ -1280,12 +1419,6 @@
     <mergeCell ref="B6:M6"/>
     <mergeCell ref="B7:M7"/>
     <mergeCell ref="B9:M9"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="F1:G1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>